<commit_message>
ein paar Integrationstests geschrieben
</commit_message>
<xml_diff>
--- a/Testdokumentation/IntegrationsTestsLeonid.xlsx
+++ b/Testdokumentation/IntegrationsTestsLeonid.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anony\Documents\Uni\TicTacToeamprojekt\Testdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4593F66D-E2F8-4ABA-B8FD-2ACA45CF5598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951C24FC-2CFB-43F7-92FF-F3439AA04ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Gerätespecs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="239">
   <si>
     <t>Leonid Surface</t>
   </si>
@@ -525,13 +538,226 @@
   </si>
   <si>
     <t>Firefox for Ubuntu 121.0 (64 Bit)</t>
+  </si>
+  <si>
+    <t>----------------------------------------------------------------------------------------old</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit "X" belegt. Der Graph rechts wird aktualisiert.</t>
+  </si>
+  <si>
+    <t>Das angeklickte Feld wird mit "O" belegt.</t>
+  </si>
+  <si>
+    <t>Die Buttons "Play" und "NextMove" sind ausgegraut. Der Graph zeigt keine Gewichte an. Über dem Spielfeld wird "X: Mensch" und "O: Mensch" angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer versucht den Slider zu verschieben.</t>
+  </si>
+  <si>
+    <t>Der Slider lässt sich nicht verschieben</t>
+  </si>
+  <si>
+    <t>Das Spielergebnis wird angezeigt: "Unentschieden!". Ein Button erscheint (Weiter).</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf "Weiter"</t>
+  </si>
+  <si>
+    <t>Der Startbildschirm wird angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Navigationssymbol "Einstellungen".</t>
+  </si>
+  <si>
+    <t>Der Einstellungen-Bildschirm wird angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt "Automatische Belohnung" aus.</t>
+  </si>
+  <si>
+    <t>Automatische Belohnung wird ausgewählt</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Navigationssymbol "Spiel" und dann auf "Spiel starten".</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt die Spielfelder in der Reihenfolge 1,2,4,5,7 an.</t>
+  </si>
+  <si>
+    <t>Das Spielergebnis wird angezeigt: "Spieler 1 gewinnt!" (in Magenta). Ein Button erscheint (Weiter).</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt im Einstellungen-Bildschirm zusätzlich "Start überspringen" aus und startet ein neues Spiel.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 1.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 2.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 4.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 5.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 8.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 7.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 3.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 6.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf dem Spielfeld auf das Feld 9.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt die Spielfelder in der Reihenfolge 1,2,4,5,9,8 an.</t>
+  </si>
+  <si>
+    <t>Das Spielergebnis wird angezeigt: "Spieler 2 gewinnt!" (in Blau). Ein Button erscheint (Weiter).</t>
+  </si>
+  <si>
+    <t>Der Spielbildschirm wird weiterhin angezeigt, aber der Spielstand ist resettet.</t>
+  </si>
+  <si>
+    <t>Der Einstellungen-Bildschirm wird angezeigt. Die beiden Optionen sind immer noch ausgewählt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer deaktiviert die Option "Automatische Belohnung", wechselt in den Spielmodus und spielt ein Spiel zuende</t>
+  </si>
+  <si>
+    <t>Das Spielergebnis wird angezeigt und der "Weiter"-Button erscheint.</t>
+  </si>
+  <si>
+    <t>Der Nutzer deaktiviert im Einstellungen-Bildschirm die Optionen "Automatische Belohnung" und "Start überspringen" und spielt ein weitere Spiel bis zum Ende</t>
+  </si>
+  <si>
+    <t>Test: Spiel mit zwei Menschen, Unentschieden und Bildschirme überspringen.</t>
+  </si>
+  <si>
+    <t>Alternativen</t>
+  </si>
+  <si>
+    <t>Der Nutzer startet ein Spiel (Mensch gegen Mensch).</t>
+  </si>
+  <si>
+    <t>Im Graph rechts werden vier Spielkonfigurationen angezeigt: Das leere Spielfeld und drei Nachfolgekonfigurationen.</t>
+  </si>
+  <si>
+    <t>Falls Desktop: Der Nutzer hovert über alle vier Spielfelder im Graphen.</t>
+  </si>
+  <si>
+    <t>Unterhalb der Spielfelder werden für die Dauer des Hovers in einer anderen Farbe andere Spielfelder in einer Zeile angezeigt. Manchmal ist das nur ein Spielfeld, manchmal mehrere.</t>
+  </si>
+  <si>
+    <t>Der Hover-Tooltip bleibt dauerhaft angezeigt, auch wenn der Nutzer nicht mehr über das Feld hovert.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt das oberste Spielfeld im Graph an.</t>
+  </si>
+  <si>
+    <t>Der Hover-Tooltip unter dem leeren Spielfeld wird genau nicht angezeigt, solange der Nutzer über das andere Spielfeld hovert. In dieser Zeit wird ein Tooltip für das andere Spielfeld angezeigt.</t>
+  </si>
+  <si>
+    <t>Es wird nur noch ein Hover-Tooltip für das angeklickte Spielfeld dauerhaft angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt erneut auf das Spielfeld unten in der Mitte-</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf das Spielfeld unten in der Mitte im Graph.</t>
+  </si>
+  <si>
+    <t>Es wird kein Hover-Tooltip mehr angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer führt einen Zug im Spielfeld aus oder lässt eine KI einen Zug ausführen.</t>
+  </si>
+  <si>
+    <t>Falls Desktop: Der Nutzer hovert über eines der anderen Spielfelder.</t>
+  </si>
+  <si>
+    <t>Falls Desktop: Der Nutzer hovert über eines der neuen und über eines der alten Spielfelder im Graph.</t>
+  </si>
+  <si>
+    <t>Es wird jeweils ein Hover-Tooltip angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf eines der neuen und auf eines der alten Spielfelder im Graph.</t>
+  </si>
+  <si>
+    <t>Es wird jeweils ein dauerhafter Hover-Tooltip angezeigt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt im "Einstellungen"-Menü die Optionen "Automatische Belohnung" und "Start überspringen" aus.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt im "Spiel"-Menü für beide Spieler die KI "KI-Elimination" aus und startet das Spiel.</t>
+  </si>
+  <si>
+    <t>Der Spiel/Graph-Bildschirm wird angezeigt</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt so lange auf das "nächster Zug"-Feld, bis das Spiel vorbei ist.</t>
+  </si>
+  <si>
+    <t>Es wird für ein paar Sekunden das Spielergebnis angezeigt, dann wird der Spiel/Graph-Bildschirm zurückgesetzt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer schiebt den Geschwindigkeitsslider auf das Maximum und klickt so lange auf das "nächster Zug"-Feld, bis das Spiel vorbei ist.</t>
+  </si>
+  <si>
+    <t>Nach dem letzten Zug einer KI wird sofort der Spiel/Graph-Bildschirm zurückgesetzt, ohne dass das Spielergebnis sichtbar ist.</t>
+  </si>
+  <si>
+    <t>Der Nutzer schiebt den Geschwindigkeitsslider auf das Minimum und klickt so lange auf das "nächster Zug"-Feld, bis das Spiel vorbei ist.</t>
+  </si>
+  <si>
+    <t>Es wird für ein einige Sekunden das Spielergebnis angezeigt, dann wird der Spiel/Graph-Bildschirm zurückgesetzt.</t>
+  </si>
+  <si>
+    <t>Der Nutzer schiebt den Geschwindigkeitsslider auf eine mittlere Position.</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt in den Einstellungen die Option "Automatische Belohnung" ab.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf "Belohnen".</t>
+  </si>
+  <si>
+    <t>Der Spiel/Graph-Bildschirm wird zurückgesetzt, der "Play"-Button ist weiter aktiv und die Kis beginnen wieder Züge zu machen.</t>
+  </si>
+  <si>
+    <t>Der Nutzer klickt auf den "Play"-Button und wartet bis das Spiel vorbei ist.</t>
+  </si>
+  <si>
+    <t>Das Spielergebnis wird angezeigt und zwei Buttons "Belohnen" und "Überspringen". Im Graph werden die Kanten des Pfads vom letzten Knoten (welcher dem Spielfeld entspricht) zum Wurzelknoten hervorgehoben. Die dazu passenden Labels ändern ihre Farbe auf Orange.</t>
+  </si>
+  <si>
+    <t>Die beiden Buttons werden durch einen Button "Weiter" ersetzt. Der Pfad ist nicht mehr hervorgehoben.</t>
+  </si>
+  <si>
+    <t>Belohnungsbildschirm überspringen mit Kis, History-Hervorhebung</t>
+  </si>
+  <si>
+    <t>Eliminations-Belohnung beider Kis</t>
+  </si>
+  <si>
+    <t>Der Nutzer wählt für Spieler 1 die KI "KI-Elimination" aus, für Spieler zwei die KI "KI-Elimination v2.0" und startet das Spiel.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +777,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -580,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,6 +825,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -896,9 +1133,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B179"/>
+  <dimension ref="A1:B245"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -906,1117 +1145,1512 @@
     <col min="2" max="2" width="145.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B44" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B45" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B65" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B66" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="67" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B67" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="68" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B68" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>73</v>
-      </c>
-      <c r="B48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>84</v>
-      </c>
-      <c r="B62" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>31</v>
+      </c>
+      <c r="B71" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>35</v>
+      </c>
+      <c r="B73" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>37</v>
+      </c>
+      <c r="B74" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>39</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>41</v>
+      </c>
+      <c r="B76" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>59</v>
+        <v>39</v>
+      </c>
+      <c r="B77" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="80" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>92</v>
+      <c r="A80" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>48</v>
+      </c>
+      <c r="B81" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="B82" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>48</v>
+      </c>
+      <c r="B83" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="B88" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>57</v>
+      </c>
+      <c r="B89" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>99</v>
+      <c r="A92" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="B94" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
-      </c>
-      <c r="B96" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>102</v>
+      <c r="A98" t="s">
+        <v>64</v>
+      </c>
+      <c r="B98" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>103</v>
+        <v>64</v>
+      </c>
+      <c r="B99" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="B100" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>65</v>
+      </c>
+      <c r="B101" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>106</v>
+      <c r="A104" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>107</v>
-      </c>
-    </row>
+        <v>27</v>
+      </c>
+      <c r="B106" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>95</v>
-      </c>
-      <c r="B108" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A108" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>71</v>
+      </c>
+      <c r="B109" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>108</v>
+      <c r="A110" t="s">
+        <v>73</v>
+      </c>
+      <c r="B110" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>103</v>
+        <v>73</v>
+      </c>
+      <c r="B111" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>48</v>
+        <v>75</v>
+      </c>
+      <c r="B112" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>109</v>
+        <v>33</v>
+      </c>
+      <c r="B113" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>110</v>
+      <c r="A116" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B117" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="B118" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>114</v>
-      </c>
-      <c r="B119" t="s">
-        <v>115</v>
-      </c>
-    </row>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>116</v>
+      <c r="A120" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>81</v>
-      </c>
-      <c r="B121" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B123" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B125" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>119</v>
+        <v>73</v>
+      </c>
+      <c r="B126" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>120</v>
-      </c>
-      <c r="B127" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>122</v>
-      </c>
-      <c r="B128" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>123</v>
-      </c>
-      <c r="B130" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>59</v>
+      </c>
+      <c r="B129" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>124</v>
+      <c r="A132" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2"/>
-      <c r="B133" t="s">
-        <v>125</v>
+      <c r="A133" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>126</v>
-      </c>
-      <c r="B134" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>128</v>
-      </c>
-      <c r="B135" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>130</v>
-      </c>
-      <c r="B136" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>132</v>
-      </c>
-      <c r="B137" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>134</v>
-      </c>
-      <c r="B138" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>126</v>
-      </c>
-      <c r="B139" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>136</v>
-      </c>
-      <c r="B140" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="B141" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>138</v>
-      </c>
-      <c r="B142" t="s">
-        <v>139</v>
-      </c>
-    </row>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>134</v>
-      </c>
-      <c r="B143" t="s">
-        <v>140</v>
+      <c r="A143" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>141</v>
-      </c>
-      <c r="B144" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>48</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B147" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="149" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>148</v>
-      </c>
-      <c r="B150" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
-      </c>
-      <c r="B151" t="s">
-        <v>151</v>
+        <v>48</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
       <c r="B153" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>154</v>
-      </c>
-      <c r="B154" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="156" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>156</v>
+      <c r="A156" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>47</v>
-      </c>
-    </row>
+        <v>95</v>
+      </c>
+      <c r="B159" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>33</v>
-      </c>
-      <c r="B161" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A161" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="163" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
-        <v>159</v>
+      <c r="A163" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>160</v>
-      </c>
-      <c r="B164" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="B165" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>162</v>
-      </c>
-    </row>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="167" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>39</v>
-      </c>
-      <c r="B167" t="s">
-        <v>40</v>
+      <c r="A167" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>41</v>
-      </c>
-      <c r="B168" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>39</v>
-      </c>
-      <c r="B169" t="s">
-        <v>161</v>
+        <v>48</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>44</v>
-      </c>
-      <c r="B170" t="s">
-        <v>163</v>
+        <v>107</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="B171" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>162</v>
-      </c>
-    </row>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="173" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>39</v>
-      </c>
-      <c r="B173" t="s">
-        <v>164</v>
+      <c r="A173" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>27</v>
-      </c>
-      <c r="B174" t="s">
-        <v>161</v>
+        <v>103</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>47</v>
-      </c>
-      <c r="B175" t="s">
-        <v>163</v>
+        <v>48</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>95</v>
+      </c>
+      <c r="B177" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>111</v>
+      </c>
+      <c r="B180" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>33</v>
+      </c>
+      <c r="B181" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>114</v>
+      </c>
+      <c r="B182" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>81</v>
+      </c>
+      <c r="B184" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>81</v>
+      </c>
+      <c r="B186" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>81</v>
+      </c>
+      <c r="B188" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>120</v>
+      </c>
+      <c r="B190" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>122</v>
+      </c>
+      <c r="B191" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>123</v>
+      </c>
+      <c r="B193" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2"/>
+      <c r="B196" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>126</v>
+      </c>
+      <c r="B197" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>128</v>
+      </c>
+      <c r="B198" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>130</v>
+      </c>
+      <c r="B199" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>132</v>
+      </c>
+      <c r="B200" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>134</v>
+      </c>
+      <c r="B201" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>126</v>
+      </c>
+      <c r="B202" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>136</v>
+      </c>
+      <c r="B203" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>130</v>
+      </c>
+      <c r="B204" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>138</v>
+      </c>
+      <c r="B205" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>134</v>
+      </c>
+      <c r="B206" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>141</v>
+      </c>
+      <c r="B207" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>145</v>
+      </c>
+      <c r="B210" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>148</v>
+      </c>
+      <c r="B213" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>150</v>
+      </c>
+      <c r="B214" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>152</v>
+      </c>
+      <c r="B216" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>154</v>
+      </c>
+      <c r="B217" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>33</v>
+      </c>
+      <c r="B224" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>160</v>
+      </c>
+      <c r="B227" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>44</v>
+      </c>
+      <c r="B228" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>39</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B230" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="231" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>41</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B231" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="232" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>39</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B232" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>44</v>
+      </c>
+      <c r="B233" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>47</v>
+      </c>
+      <c r="B234" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>39</v>
+      </c>
+      <c r="B236" t="s">
         <v>164</v>
       </c>
     </row>
+    <row r="237" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>27</v>
+      </c>
+      <c r="B237" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>47</v>
+      </c>
+      <c r="B238" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>39</v>
+      </c>
+      <c r="B240" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>41</v>
+      </c>
+      <c r="B241" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>39</v>
+      </c>
+      <c r="B242" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2027,7 +2661,7 @@
   </sheetPr>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
@@ -2169,6 +2803,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Q3:S3"/>
@@ -2185,14 +2827,6 @@
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>